<commit_message>
data - Se agrego el excell que actualiza los proyectos
</commit_message>
<xml_diff>
--- a/data/teamDB2.xlsx
+++ b/data/teamDB2.xlsx
@@ -397,7 +397,7 @@
     <t xml:space="preserve">astridlun</t>
   </si>
   <si>
-    <t xml:space="preserve">My research interest is conservation genetics/conservation genomics of vulnerable or endangered species as a tool for designing strategies to allow their persistence in the ecosystem. Currently, I focus my work on the loggerhead turtle (Caretta caretta), on the one hand I study the new nesting sites on the Spanish coast, and the relationship of these patterns with climate change. On the other hand, I have designed a genomic baseline that includes data from 3 Regional Management Units: North East Atlantic, North West Atlantic and Mediterranean for the assignment of individuals sampled in Mediterranean foraging areas.</t>
+    <t xml:space="preserve">My research interest is conservation genetics/conservation genomics of vulnerable or endangered species as a tool for designing strategies to allow their persistence in the ecosystem. Currently, I focus my work on the loggerhead turtle (Caretta caretta), on the one hand I study the new nesting sites on the Spanish coast, and the relationship of these patterns with climate change. On the other hand, I have designed a genomic baseline that includes data from 3 Regional Management Units: North East Atlantic, North West Atlantic and Mediterranean for the assignment of individuals sampled in Mediterranean foraging areas. </t>
   </si>
   <si>
     <t xml:space="preserve">Vanessa Arranz</t>
@@ -986,7 +986,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -994,7 +994,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1038,7 +1038,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1134,7 +1134,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1142,7 +1142,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1170,11 +1170,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1186,7 +1186,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1218,11 +1218,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1558,10 +1558,10 @@
   </sheetPr>
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
-      <selection pane="bottomLeft" activeCell="P8" activeCellId="0" sqref="P8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="N21" activeCellId="0" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2773,9 +2773,9 @@
     <hyperlink ref="K10" r:id="rId18" display="http://opistobranquis.info/en/"/>
     <hyperlink ref="I11" r:id="rId19" display="https://orcid.org/0000-0002-0945-0249"/>
     <hyperlink ref="J11" r:id="rId20" display="https://scholar.google.com/citations?hl=en&amp;user=9b_b_o0AAAAJ"/>
-    <hyperlink ref="I12" r:id="rId21" display="https://orcid.org/my-orcid?orcid=0000-0003-4736-551X"/>
+    <hyperlink ref="I12" r:id="rId21" display=" https://orcid.org/my-orcid?orcid=0000-0003-4736-551X"/>
     <hyperlink ref="J12" r:id="rId22" display="https://scholar.google.com/citations?user=aH4kBdgAAAAJ&amp;hl=en"/>
-    <hyperlink ref="M12" r:id="rId23" display="https://www.linkedin.com/in/astrid-luna-9872621b5/"/>
+    <hyperlink ref="M12" r:id="rId23" display=" https://www.linkedin.com/in/astrid-luna-9872621b5/"/>
     <hyperlink ref="I13" r:id="rId24" display="https://orcid.org/0000-0002-3404-5317"/>
     <hyperlink ref="J13" r:id="rId25" display="https://scholar.google.com/citations?user=-1eos5cAAAAJ&amp;hl=en"/>
     <hyperlink ref="K13" r:id="rId26" display="https://echinoadaptive.wixsite.com/adaptive-team"/>
@@ -2794,12 +2794,13 @@
     <hyperlink ref="J20" r:id="rId39" display="https://scholar.google.es/citations?user=dVED18oAAAAJ&amp;hl=es&amp;oi=sra"/>
     <hyperlink ref="I21" r:id="rId40" display="https://orcid.org/0009-0006-1599-9357"/>
     <hyperlink ref="J21" r:id="rId41" display="https://scholar.google.com/citations?hl=es&amp;user=37txp4oAAAAJ"/>
-    <hyperlink ref="I22" r:id="rId42" display="https://orcid.org/0009-0006-7678-9337"/>
-    <hyperlink ref="J22" r:id="rId43" display="https://scholar.google.es/citations?view_op=list_works&amp;hl=en&amp;user=xZ33otQAAAAJ"/>
-    <hyperlink ref="I23" r:id="rId44" display="https://orcid.org/0009-0000-5937-2819"/>
-    <hyperlink ref="J23" r:id="rId45" display="https://scholar.google.es/citations?view_op=list_works&amp;hl=es&amp;user=Pp7ie7cAAAAJ&amp;gmla=AOv-ny9xwCSiAxoadH38LpB1MxFbZ7kuWGNiUjVgaDW9FSMpFBXI2s0K4SKQAatpg3MsY3N05P-ibvlYBq8dAq2pMI_YRiVOtMZubq9aSukIedzZi2TmXQ2b_gh56CPCphLUog8"/>
-    <hyperlink ref="I25" r:id="rId46" display="https://orcid.org/0009-0003-7746-2035"/>
-    <hyperlink ref="J25" r:id="rId47" display="https://scholar.google.com/citations?user=YdHnkqUAAAAJ&amp;hl=en"/>
+    <hyperlink ref="N21" r:id="rId42" display="https://bsky.app/profile/ainhoalopez.bsky.social"/>
+    <hyperlink ref="I22" r:id="rId43" display="https://orcid.org/0009-0006-7678-9337"/>
+    <hyperlink ref="J22" r:id="rId44" display="https://scholar.google.es/citations?view_op=list_works&amp;hl=en&amp;user=xZ33otQAAAAJ"/>
+    <hyperlink ref="I23" r:id="rId45" display="https://orcid.org/0009-0000-5937-2819"/>
+    <hyperlink ref="J23" r:id="rId46" display="https://scholar.google.es/citations?view_op=list_works&amp;hl=es&amp;user=Pp7ie7cAAAAJ&amp;gmla=AOv-ny9xwCSiAxoadH38LpB1MxFbZ7kuWGNiUjVgaDW9FSMpFBXI2s0K4SKQAatpg3MsY3N05P-ibvlYBq8dAq2pMI_YRiVOtMZubq9aSukIedzZi2TmXQ2b_gh56CPCphLUog8"/>
+    <hyperlink ref="I25" r:id="rId47" display="https://orcid.org/0009-0003-7746-2035"/>
+    <hyperlink ref="J25" r:id="rId48" display="https://scholar.google.com/citations?user=YdHnkqUAAAAJ&amp;hl=en"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2809,7 +2810,7 @@
     <oddFooter/>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId48"/>
+    <tablePart r:id="rId49"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>